<commit_message>
working on the ripple introduction
</commit_message>
<xml_diff>
--- a/ripple/chess13a_analysis/085_ver3.xlsx
+++ b/ripple/chess13a_analysis/085_ver3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="255" windowWidth="16380" windowHeight="8190" tabRatio="382" activeTab="1"/>
+    <workbookView xWindow="705" yWindow="255" windowWidth="16380" windowHeight="8190" tabRatio="382" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="everything" sheetId="1" r:id="rId1"/>
@@ -4542,8 +4542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4558,7 +4558,7 @@
     <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125"/>
+    <col min="12" max="12" width="6.5703125" customWidth="1"/>
     <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -8008,7 +8008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>